<commit_message>
ajustado bug ao salvar clientes na planilha
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Clientes" sheetId="2" r:id="rId2"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,19 +397,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData/>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
@@ -444,42 +430,48 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2</v>
+        <v>joao</v>
       </c>
       <c r="B2" t="str">
-        <v>3</v>
+        <v>12312312</v>
       </c>
       <c r="C2" t="str">
-        <v>6</v>
+        <v>0000000000</v>
       </c>
       <c r="E2" t="str">
-        <v>qweqwe@qweqwe</v>
+        <v>010101010101</v>
       </c>
       <c r="F2" t="str">
-        <v>4</v>
+        <v>brunofraga@gmail.com</v>
+      </c>
+      <c r="G2" t="str">
+        <v>3332113221</v>
       </c>
       <c r="H2" t="str">
-        <v>5</v>
+        <v>mato grande</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>123</v>
+        <v>bruno</v>
       </c>
       <c r="B3" t="str">
-        <v>123123</v>
+        <v>Itried1993</v>
       </c>
       <c r="C3" t="str">
-        <v>123123</v>
+        <v>02370945095</v>
       </c>
       <c r="E3" t="str">
-        <v>1231!@3123</v>
+        <v>92320-195</v>
       </c>
       <c r="F3" t="str">
-        <v>12312</v>
+        <v>brunofraga@gmail.com</v>
+      </c>
+      <c r="G3" t="str">
+        <v>51989043802</v>
       </c>
       <c r="H3" t="str">
-        <v>123123</v>
+        <v>R. 3 Pinheiros I - Mato Grande</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterado nomenclatura das classes, para melhor compreensao das classes
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -474,9 +474,55 @@
         <v>R. 3 Pinheiros I - Mato Grande</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>paulo</v>
+      </c>
+      <c r="B4" t="str">
+        <v>987584</v>
+      </c>
+      <c r="C4" t="str">
+        <v>321321321</v>
+      </c>
+      <c r="E4" t="str">
+        <v>92320192</v>
+      </c>
+      <c r="F4" t="str">
+        <v>pauloroberto@gmail.com</v>
+      </c>
+      <c r="G4" t="str">
+        <v>51999875487</v>
+      </c>
+      <c r="H4" t="str">
+        <v>RUA DOS PINHAIS</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="B5" t="str">
+        <v>9918283182</v>
+      </c>
+      <c r="C5" t="str">
+        <v>91283912738216</v>
+      </c>
+      <c r="E5" t="str">
+        <v>99827371</v>
+      </c>
+      <c r="F5" t="str">
+        <v>matheus@gmail.com</v>
+      </c>
+      <c r="G5" t="str">
+        <v>120392391298</v>
+      </c>
+      <c r="H5" t="str">
+        <v>rua da topeira</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizado log console navegador
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -520,9 +520,239 @@
         <v>rua da topeira</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>roberto</v>
+      </c>
+      <c r="B6" t="str">
+        <v>123123124</v>
+      </c>
+      <c r="C6" t="str">
+        <v>991232</v>
+      </c>
+      <c r="E6" t="str">
+        <v>19123829</v>
+      </c>
+      <c r="F6" t="str">
+        <v>roberto@gmail.com</v>
+      </c>
+      <c r="G6" t="str">
+        <v>1928391823</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Rua das tropaceiras</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>bruno</v>
+      </c>
+      <c r="B7" t="str">
+        <v>12312</v>
+      </c>
+      <c r="C7" t="str">
+        <v>019230812938</v>
+      </c>
+      <c r="E7" t="str">
+        <v>819238192389</v>
+      </c>
+      <c r="F7" t="str">
+        <v>brunofraga@gmail.com</v>
+      </c>
+      <c r="G7" t="str">
+        <v>182381723</v>
+      </c>
+      <c r="H7" t="str">
+        <v>ruas das molecas</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B8" t="str">
+        <v>12312</v>
+      </c>
+      <c r="C8" t="str">
+        <v>12312312</v>
+      </c>
+      <c r="E8" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F8" t="str">
+        <v>qweqwe@qweqwe</v>
+      </c>
+      <c r="G8" t="str">
+        <v>132123123</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>joanues</v>
+      </c>
+      <c r="B9" t="str">
+        <v>1293i1923</v>
+      </c>
+      <c r="C9" t="str">
+        <v>-1203192309</v>
+      </c>
+      <c r="E9" t="str">
+        <v>123912839</v>
+      </c>
+      <c r="F9" t="str">
+        <v>joanues@gmail.com</v>
+      </c>
+      <c r="G9" t="str">
+        <v>123i912329</v>
+      </c>
+      <c r="H9" t="str">
+        <v>rua das horticias</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>maria</v>
+      </c>
+      <c r="B10" t="str">
+        <v>1923192839</v>
+      </c>
+      <c r="C10" t="str">
+        <v>39139212068</v>
+      </c>
+      <c r="E10" t="str">
+        <v>91239182938</v>
+      </c>
+      <c r="F10" t="str">
+        <v>maria@gmail.com</v>
+      </c>
+      <c r="G10" t="str">
+        <v>1923891283</v>
+      </c>
+      <c r="H10" t="str">
+        <v>rua das alamedas</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>ana luiza</v>
+      </c>
+      <c r="B11" t="str">
+        <v>SJAISJDI@@</v>
+      </c>
+      <c r="C11" t="str">
+        <v>19238912381273</v>
+      </c>
+      <c r="E11" t="str">
+        <v>9123918239</v>
+      </c>
+      <c r="F11" t="str">
+        <v>analuiza@gmail.com</v>
+      </c>
+      <c r="G11" t="str">
+        <v>192u391239182</v>
+      </c>
+      <c r="H11" t="str">
+        <v>multi dimensoses</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>leticia</v>
+      </c>
+      <c r="B12" t="str">
+        <v>98745451</v>
+      </c>
+      <c r="C12" t="str">
+        <v>91283918239</v>
+      </c>
+      <c r="E12" t="str">
+        <v>128391823981</v>
+      </c>
+      <c r="F12" t="str">
+        <v>leticia@gmail.com</v>
+      </c>
+      <c r="G12" t="str">
+        <v>19283912839</v>
+      </c>
+      <c r="H12" t="str">
+        <v>rua das corticeiras</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>joana</v>
+      </c>
+      <c r="B13" t="str">
+        <v>12381928391</v>
+      </c>
+      <c r="C13" t="str">
+        <v>1928391823</v>
+      </c>
+      <c r="E13" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F13" t="str">
+        <v>joana@gmail.com</v>
+      </c>
+      <c r="G13" t="str">
+        <v>19823918293182</v>
+      </c>
+      <c r="H13" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>francine</v>
+      </c>
+      <c r="B14" t="str">
+        <v>123912u3192</v>
+      </c>
+      <c r="C14" t="str">
+        <v>19283928391</v>
+      </c>
+      <c r="E14" t="str">
+        <v>192839123891</v>
+      </c>
+      <c r="F14" t="str">
+        <v>fran@gmail.com</v>
+      </c>
+      <c r="G14" t="str">
+        <v>1923819283</v>
+      </c>
+      <c r="H14" t="str">
+        <v>rua tapajos</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>joselito</v>
+      </c>
+      <c r="B15" t="str">
+        <v>12319238</v>
+      </c>
+      <c r="C15" t="str">
+        <v>1923891283</v>
+      </c>
+      <c r="E15" t="str">
+        <v>1923912839</v>
+      </c>
+      <c r="F15" t="str">
+        <v>qweqweqweq@qweqwe</v>
+      </c>
+      <c r="G15" t="str">
+        <v>91823918293</v>
+      </c>
+      <c r="H15" t="str">
+        <v>qjwdqwhduhq</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criado estutura basica para implementacao do componente cardapio
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -750,9 +750,32 @@
         <v>qjwdqwhduhq</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>sandro</v>
+      </c>
+      <c r="B16" t="str">
+        <v>1238192312</v>
+      </c>
+      <c r="C16" t="str">
+        <v>91823918239</v>
+      </c>
+      <c r="E16" t="str">
+        <v>1928391823</v>
+      </c>
+      <c r="F16" t="str">
+        <v>hduhwdq@djuqwhduqh</v>
+      </c>
+      <c r="G16" t="str">
+        <v>1283128312</v>
+      </c>
+      <c r="H16" t="str">
+        <v>rua das alamedas</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renomiado componentes de Cardapio para Pedido / Criado classe pedido no backend
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -773,9 +773,32 @@
         <v>rua das alamedas</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>lucas</v>
+      </c>
+      <c r="B17" t="str">
+        <v>asdasdas</v>
+      </c>
+      <c r="C17" t="str">
+        <v>asdasdas</v>
+      </c>
+      <c r="E17" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F17" t="str">
+        <v>joanues@gmail.com</v>
+      </c>
+      <c r="G17" t="str">
+        <v>12312312312</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionado modal ao clicar no botao cadastro, modal ja ajustado
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -796,9 +796,32 @@
         <v>Rua 3 Pinheiros I, 27</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B18" t="str">
+        <v>123123123</v>
+      </c>
+      <c r="C18" t="str">
+        <v>02370945095</v>
+      </c>
+      <c r="E18" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F18" t="str">
+        <v>joanues@gmail.com</v>
+      </c>
+      <c r="G18" t="str">
+        <v>5154548</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionado por prop funcao de fechar modal da tela de cadastro, apos cadastrar o usuario o modal fecha sozinho
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -819,9 +819,55 @@
         <v>Rua 3 Pinheiros I, 27</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B19" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C19" t="str">
+        <v>123123</v>
+      </c>
+      <c r="E19" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F19" t="str">
+        <v>qweqweqweq@qweqwe</v>
+      </c>
+      <c r="G19" t="str">
+        <v>123123123123</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B20" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C20" t="str">
+        <v>123123</v>
+      </c>
+      <c r="E20" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F20" t="str">
+        <v>1231!@3123</v>
+      </c>
+      <c r="G20" t="str">
+        <v>123123</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modais foram separados, tela de login configurado mas ainda sem inteligencia de login
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -865,9 +865,55 @@
         <v>Rua 3 Pinheiros I, 27</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B21" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C21" t="str">
+        <v>123123</v>
+      </c>
+      <c r="E21" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F21" t="str">
+        <v>12312312@123123</v>
+      </c>
+      <c r="G21" t="str">
+        <v>123123</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B22" t="str">
+        <v>12312312</v>
+      </c>
+      <c r="C22" t="str">
+        <v>12312312</v>
+      </c>
+      <c r="E22" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F22" t="str">
+        <v>joanues@gmail.com</v>
+      </c>
+      <c r="G22" t="str">
+        <v>12312312</v>
+      </c>
+      <c r="H22" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H22"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado o paramentro para enviar a data e hora da requisicao
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -911,9 +911,124 @@
         <v>Rua 3 Pinheiros I, 27</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B23" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C23" t="str">
+        <v>023.709.450-95</v>
+      </c>
+      <c r="E23" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F23" t="str">
+        <v>bruno@gmail.com</v>
+      </c>
+      <c r="G23" t="str">
+        <v>51989043802</v>
+      </c>
+      <c r="H23" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B24" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C24" t="str">
+        <v>3123123</v>
+      </c>
+      <c r="E24" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F24" t="str">
+        <v>bruno@gmail.com</v>
+      </c>
+      <c r="G24" t="str">
+        <v>51989043802</v>
+      </c>
+      <c r="H24" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B25" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C25" t="str">
+        <v>123123</v>
+      </c>
+      <c r="E25" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F25" t="str">
+        <v>bruno@gmail.com</v>
+      </c>
+      <c r="G25" t="str">
+        <v>51989043802</v>
+      </c>
+      <c r="H25" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B26" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C26" t="str">
+        <v>023.709.450-95</v>
+      </c>
+      <c r="E26" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F26" t="str">
+        <v>bruno@gmail.com</v>
+      </c>
+      <c r="G26" t="str">
+        <v>51989043802</v>
+      </c>
+      <c r="H26" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>BRUNO DE FRAGA</v>
+      </c>
+      <c r="B27" t="str">
+        <v>123123</v>
+      </c>
+      <c r="C27" t="str">
+        <v>4123123</v>
+      </c>
+      <c r="E27" t="str">
+        <v>92320-195</v>
+      </c>
+      <c r="F27" t="str">
+        <v>bruno@gmail.com</v>
+      </c>
+      <c r="G27" t="str">
+        <v>51989043802</v>
+      </c>
+      <c r="H27" t="str">
+        <v>Rua 3 Pinheiros I, 27</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionado funcao para nao deixar verificar o pedido sem antes logar
</commit_message>
<xml_diff>
--- a/Sitema_Pedidos/Backend/clientes.xlsx
+++ b/Sitema_Pedidos/Backend/clientes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1026,9 +1026,32 @@
         <v>Rua 3 Pinheiros I, 27</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>francine benedetto</v>
+      </c>
+      <c r="B28" t="str">
+        <v>945833</v>
+      </c>
+      <c r="C28" t="str">
+        <v>85081450049</v>
+      </c>
+      <c r="E28" t="str">
+        <v>92410480</v>
+      </c>
+      <c r="F28" t="str">
+        <v>francinebenedetto@gmail.com</v>
+      </c>
+      <c r="G28" t="str">
+        <v>51994723632</v>
+      </c>
+      <c r="H28" t="str">
+        <v>rua tapajos 50</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>